<commit_message>
update git ignore, input file notes from gus
</commit_message>
<xml_diff>
--- a/update_2018_notes.xlsx
+++ b/update_2018_notes.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21727"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{762C954E-28D2-45BB-ACCC-106F6732B974}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C892B31-A516-4242-A5FC-1F53B28B765F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="input_file_dictionary" sheetId="5" r:id="rId1"/>
@@ -310,9 +310,6 @@
     <t>Questions?</t>
   </si>
   <si>
-    <t>Number of: fields, irrigation wells, stress periods, rows, and columns. RD_Mult? Also specifies UCODE or PEST calibration, and which scenario is running.</t>
-  </si>
-  <si>
     <t>Effective irrigation efficiencies for flood; for alfalfa-wheel line and alfalfa-center pivot; and for pasture-wheel line and pasture-center pivot.</t>
   </si>
   <si>
@@ -338,9 +335,6 @@
   </si>
   <si>
     <t>???? Field IDs?</t>
-  </si>
-  <si>
-    <t>Daily reference ET in meters and then in inches. Why did we choose to have consistent monthly ET values? Should I preserve those during the model update, or use daily values? Should I use daily values going forward?</t>
   </si>
   <si>
     <t>Key:</t>
@@ -502,32 +496,6 @@
     <t>SVIHM.ets</t>
   </si>
   <si>
-    <r>
-      <t>Head observation file. Preamble, then, for each well, a row containing: location name, layer, row, column, number of stress periods containing an observation (listed as a negative number), an offset time from the start of the stress period (seems to be used for a structure where each location has one obselvation; it's just 0 for all of ours), row and column offset from center of cell (as fractions of cell width or height; all of ours are located in the middle of a quadrant, specified with + or - 0.25 offsets), and some extra parameters. For each observation under that well, list the unique observation identifier (built on the location name), the stress period in which the measurement was made, the number of time steps into the stress period, the head measurement (meters above mean sea level), and some extra parameters.</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> How do we connect the CASGEM ids with the DWR_2 ids in the model? Lat/long? What's the fastest way to add new wells to this file? </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Make to do list in here</t>
-    </r>
-  </si>
-  <si>
     <t>drafted with outstanding to dos</t>
   </si>
   <si>
@@ -611,6 +579,38 @@
   </si>
   <si>
     <t>Make a list of files you will need to change to accomplish the following tasks: 1) run a scenario; 2) update the hydrogeologic conceptual model; 3) extend the model period</t>
+  </si>
+  <si>
+    <t>Daily reference ET in meters and then in inches. Why did we choose to have consistent monthly ET values? Should I preserve those during the model update, or use daily values? Should I use daily values going forward? Compare ET values for monthly ref ET and daily??</t>
+  </si>
+  <si>
+    <r>
+      <t>Head observation file. Preamble, then, for each well, a row containing: location name, layer, row, column, number of stress periods containing an observation (listed as a negative number), an offset time from the start of the stress period (seems to be used for a structure where each location has one obselvation; it's just 0 for all of ours), row and column offset from center of cell (as fractions of cell width or height; all of ours are located in the middle of a quadrant, specified with + or - 0.25 offsets), and some extra parameters. For each observation under that well, list the unique observation identifier (built on the location name), the stress period in which the measurement was made, the number of time steps into the stress period, the head measurement (meters above mean sea level), and some extra parameters.</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> How do we connect the CASGEM ids with the DWR_2 ids in the model? Locate them in GIS Lat/long? What's the fastest way to add new wells to this file? </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Make to do list in here</t>
+    </r>
+  </si>
+  <si>
+    <t>Number of: fields, irrigation wells, stress periods, rows, and columns. RD_Mult? Scales the Root Depth initial value. Also specifies UCODE or PEST calibration, and which scenario is running.</t>
   </si>
 </sst>
 </file>
@@ -1885,8 +1885,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4586B933-D340-49CB-AB4A-230CE00A6B42}">
   <dimension ref="A1:G93"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="F36" sqref="F36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1903,39 +1903,39 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B1" s="25" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C1" s="25"/>
       <c r="D1" s="23" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="E1" s="13" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="G1" s="12"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="D2" s="24" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="E2" s="11" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="D3" s="17" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="E3" s="10" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="D4" s="16" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="E4" s="14" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -1947,7 +1947,7 @@
       </c>
       <c r="C6" s="26"/>
       <c r="D6" s="27" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="E6" s="27" t="s">
         <v>91</v>
@@ -1965,7 +1965,7 @@
       </c>
       <c r="C7" s="18"/>
       <c r="D7" s="16" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="E7" s="19"/>
       <c r="F7" s="20" t="s">
@@ -1981,7 +1981,7 @@
       </c>
       <c r="C8" s="18"/>
       <c r="D8" s="16" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="E8" s="21"/>
       <c r="F8" s="20" t="s">
@@ -1997,7 +1997,7 @@
       </c>
       <c r="C9" s="18"/>
       <c r="D9" s="23" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="E9" s="18"/>
       <c r="F9" s="20" t="s">
@@ -2013,7 +2013,7 @@
       </c>
       <c r="C10" s="18"/>
       <c r="D10" s="23" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="E10" s="21"/>
       <c r="F10" s="20" t="s">
@@ -2029,14 +2029,14 @@
       </c>
       <c r="C11" s="18"/>
       <c r="D11" s="16" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="E11" s="18"/>
       <c r="F11" s="20" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A12" s="18" t="s">
         <v>84</v>
       </c>
@@ -2045,11 +2045,11 @@
       </c>
       <c r="C12" s="18"/>
       <c r="D12" s="23" t="s">
-        <v>116</v>
-      </c>
-      <c r="E12" s="21"/>
+        <v>114</v>
+      </c>
+      <c r="E12" s="28"/>
       <c r="F12" s="20" t="s">
-        <v>92</v>
+        <v>168</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -2061,11 +2061,11 @@
       </c>
       <c r="C13" s="18"/>
       <c r="D13" s="16" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="E13" s="18"/>
       <c r="F13" s="20" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -2077,11 +2077,11 @@
       </c>
       <c r="C14" s="18"/>
       <c r="D14" s="23" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="E14" s="18"/>
       <c r="F14" s="20" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -2093,11 +2093,11 @@
       </c>
       <c r="C15" s="18"/>
       <c r="D15" s="23" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="E15" s="21"/>
       <c r="F15" s="20" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -2109,11 +2109,11 @@
       </c>
       <c r="C16" s="18"/>
       <c r="D16" s="23" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="E16" s="18"/>
       <c r="F16" s="20" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -2125,11 +2125,11 @@
       </c>
       <c r="C17" s="18"/>
       <c r="D17" s="16" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="E17" s="21"/>
       <c r="F17" s="20" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
@@ -2141,11 +2141,11 @@
       </c>
       <c r="C18" s="18"/>
       <c r="D18" s="16" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="E18" s="18"/>
       <c r="F18" s="20" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -2157,11 +2157,11 @@
       </c>
       <c r="C19" s="18"/>
       <c r="D19" s="16" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="E19" s="18"/>
       <c r="F19" s="20" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
@@ -2173,11 +2173,11 @@
       </c>
       <c r="C20" s="18"/>
       <c r="D20" s="24" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="E20" s="18"/>
       <c r="F20" s="20" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
@@ -2189,11 +2189,11 @@
       </c>
       <c r="C21" s="18"/>
       <c r="D21" s="16" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="E21" s="19"/>
       <c r="F21" s="20" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -2205,11 +2205,11 @@
       </c>
       <c r="C22" s="18"/>
       <c r="D22" s="24" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="E22" s="22"/>
       <c r="F22" s="20" t="s">
-        <v>102</v>
+        <v>166</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
@@ -2221,11 +2221,11 @@
       </c>
       <c r="C23" s="18"/>
       <c r="D23" s="17" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="E23" s="19"/>
       <c r="F23" s="20" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
@@ -2237,27 +2237,27 @@
       </c>
       <c r="C24" s="18"/>
       <c r="D24" s="17" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="E24" s="19"/>
       <c r="F24" s="20" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A25" s="20" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B25" s="18" t="s">
         <v>33</v>
       </c>
       <c r="C25" s="18"/>
       <c r="D25" s="29" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="E25" s="18"/>
       <c r="F25" s="20" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
@@ -2269,11 +2269,11 @@
       </c>
       <c r="C26" s="18"/>
       <c r="D26" s="16" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="E26" s="21"/>
       <c r="F26" s="20" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
@@ -2285,11 +2285,11 @@
       </c>
       <c r="C27" s="18"/>
       <c r="D27" s="16" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="E27" s="21"/>
       <c r="F27" s="20" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="115.2" x14ac:dyDescent="0.3">
@@ -2301,11 +2301,11 @@
       </c>
       <c r="C28" s="18"/>
       <c r="D28" s="16" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="E28" s="21"/>
       <c r="F28" s="20" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="29" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -2317,11 +2317,11 @@
       </c>
       <c r="C29" s="18"/>
       <c r="D29" s="16" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="E29" s="21"/>
       <c r="F29" s="20" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="30" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -2333,313 +2333,313 @@
       </c>
       <c r="C30" s="18"/>
       <c r="D30" s="16" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="E30" s="18"/>
       <c r="F30" s="20" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" s="28" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B31" s="16" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C31" s="16"/>
       <c r="D31" s="29" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="E31" s="16"/>
       <c r="F31" s="30"/>
     </row>
     <row r="32" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A32" s="28" t="s">
+        <v>120</v>
+      </c>
+      <c r="B32" s="16" t="s">
         <v>122</v>
       </c>
-      <c r="B32" s="16" t="s">
-        <v>124</v>
-      </c>
       <c r="C32" s="16" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="D32" s="16" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="E32" s="31"/>
       <c r="F32" s="30" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="33" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A33" s="28" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B33" s="16" t="s">
         <v>44</v>
       </c>
       <c r="C33" s="16" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="D33" s="29" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="E33" s="16"/>
       <c r="F33" s="30" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="34" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A34" s="28" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B34" s="16" t="s">
         <v>46</v>
       </c>
       <c r="C34" s="16" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="D34" s="29" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="E34" s="16"/>
       <c r="F34" s="30" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35" s="28" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B35" s="16" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C35" s="16"/>
       <c r="D35" s="16" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="E35" s="16"/>
       <c r="F35" s="30" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="36" spans="1:6" ht="72" x14ac:dyDescent="0.3">
       <c r="A36" s="28" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B36" s="16" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C36" s="16" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="D36" s="16" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="E36" s="31"/>
       <c r="F36" s="30" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="37" spans="1:6" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A37" s="28" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B37" s="16" t="s">
         <v>51</v>
       </c>
       <c r="C37" s="16" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="D37" s="33" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="E37" s="31"/>
       <c r="F37" s="30" t="s">
-        <v>144</v>
+        <v>167</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38" s="28" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B38" s="16" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C38" s="16" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="D38" s="16" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="E38" s="16"/>
       <c r="F38" s="30" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39" s="28" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B39" s="16" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C39" s="16" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="D39" s="16" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="E39" s="16"/>
       <c r="F39" s="30" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A40" s="28"/>
       <c r="B40" s="16" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="C40" s="16"/>
       <c r="D40" s="16"/>
       <c r="E40" s="16" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="F40" s="30"/>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A41" s="28" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B41" s="16" t="s">
         <v>45</v>
       </c>
       <c r="C41" s="16" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="D41" s="29" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="E41" s="16"/>
       <c r="F41" s="30" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
     </row>
     <row r="42" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A42" s="28" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B42" s="16" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C42" s="16" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="D42" s="16" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="E42" s="16"/>
       <c r="F42" s="30" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A43" s="28"/>
       <c r="B43" s="16" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C43" s="16" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="D43" s="16" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="E43" s="16"/>
       <c r="F43" s="30" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="44" spans="1:6" ht="72" x14ac:dyDescent="0.3">
       <c r="A44" s="28" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B44" s="16" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C44" s="16" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="D44" s="16" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="E44" s="31"/>
       <c r="F44" s="30" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A45" s="28" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B45" s="16" t="s">
         <v>47</v>
       </c>
       <c r="C45" s="16"/>
       <c r="D45" s="16" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="E45" s="16"/>
       <c r="F45" s="30" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A46" s="28" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B46" s="16" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C46" s="16"/>
       <c r="D46" s="16" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="E46" s="16"/>
       <c r="F46" s="30" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A47" s="28" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B47" s="16" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C47" s="16"/>
       <c r="D47" s="16" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="E47" s="31"/>
       <c r="F47" s="30" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A48" s="28" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B48" s="16" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C48" s="16"/>
       <c r="D48" s="16" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="E48" s="31"/>
       <c r="F48" s="30" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
     </row>
     <row r="74" spans="6:6" x14ac:dyDescent="0.3">
@@ -2713,7 +2713,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17E60BD9-E4DA-475A-8F4C-03B41D8829BF}">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
@@ -2721,15 +2721,15 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="B3" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
solve hob run error
</commit_message>
<xml_diff>
--- a/update_2018_notes.xlsx
+++ b/update_2018_notes.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21727"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C892B31-A516-4242-A5FC-1F53B28B765F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F7601BD-67E7-423D-9A40-BA51CE0FCF54}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2172" yWindow="2088" windowWidth="19932" windowHeight="8976" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="input_file_dictionary" sheetId="5" r:id="rId1"/>
@@ -1885,8 +1885,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4586B933-D340-49CB-AB4A-230CE00A6B42}">
   <dimension ref="A1:G93"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="F36" sqref="F36"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="F37" sqref="F37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2741,8 +2741,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H339"/>
   <sheetViews>
-    <sheetView topLeftCell="A311" workbookViewId="0">
-      <selection activeCell="H337" sqref="H337"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2831,7 +2831,7 @@
         <v>2</v>
       </c>
       <c r="G3" s="6">
-        <f t="shared" ref="G3:G66" si="0">DATE(B3,D3,1)</f>
+        <f>DATE(B3,D3,1)</f>
         <v>33178</v>
       </c>
       <c r="H3">
@@ -2859,7 +2859,7 @@
         <v>3</v>
       </c>
       <c r="G4" s="6">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="G3:G66" si="0">DATE(B4,D4,1)</f>
         <v>33208</v>
       </c>
       <c r="H4">

</xml_diff>

<commit_message>
fix fail-on-penultimate-stress-period bug. clean folders
</commit_message>
<xml_diff>
--- a/update_2018_notes.xlsx
+++ b/update_2018_notes.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21727"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F7601BD-67E7-423D-9A40-BA51CE0FCF54}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B7003D2-95B0-4BA1-8F07-B245891DEE36}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2172" yWindow="2088" windowWidth="19932" windowHeight="8976" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="input_file_dictionary" sheetId="5" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="171">
   <si>
     <t>year</t>
   </si>
@@ -356,9 +356,6 @@
   </si>
   <si>
     <t>ETS input template. ETS used to simulate ET from the saturated zone. We have no parameters because we don't calibrate on ET? (but don't we? We calibrate using the kc values.) Do we not have a Data Set 2? In Data Set 4, what does INETSS mean? What are all these numbers? Starting points for ET?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Why is thickness and conductivity always 1 and 10? SFR input template. Stream-Flow Routing. Each row pertains to a "reach." Reaches belong to longer "segments." Each row contains the following info: layer, row, column, segment, reach number. Reach length, elevation, slope. Streambed thickness and conductivity (1 and 10). </t>
   </si>
   <si>
     <t xml:space="preserve">Log number (associated with Well Completion Reports), layer the well pulls from, row, column, easting and northing. </t>
@@ -611,6 +608,36 @@
   </si>
   <si>
     <t>Number of: fields, irrigation wells, stress periods, rows, and columns. RD_Mult? Scales the Root Depth initial value. Also specifies UCODE or PEST calibration, and which scenario is running.</t>
+  </si>
+  <si>
+    <t>Make a well disambiguation table</t>
+  </si>
+  <si>
+    <t>Make a cross-section-generating script: viewing the hydrogeologic conceptual model in 2D. Zones and also head values</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Why is thickness and conductivity always 1 and 10</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">? (Because the model isnt' sensitive to it.) SFR input template. Stream-Flow Routing. Each row pertains to a "reach." Reaches belong to longer "segments." Each row contains the following info: layer, row, column, segment, reach number. Reach length, elevation, slope. Streambed thickness and conductivity (1 and 10). 
+After written by SWBM: </t>
+    </r>
   </si>
 </sst>
 </file>
@@ -1885,8 +1912,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4586B933-D340-49CB-AB4A-230CE00A6B42}">
   <dimension ref="A1:G93"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="F37" sqref="F37"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1907,7 +1934,7 @@
       </c>
       <c r="C1" s="25"/>
       <c r="D1" s="23" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E1" s="13" t="s">
         <v>102</v>
@@ -1916,7 +1943,7 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="D2" s="24" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E2" s="11" t="s">
         <v>105</v>
@@ -1924,7 +1951,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="D3" s="17" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E3" s="10" t="s">
         <v>103</v>
@@ -1932,7 +1959,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="D4" s="16" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E4" s="14" t="s">
         <v>104</v>
@@ -1947,7 +1974,7 @@
       </c>
       <c r="C6" s="26"/>
       <c r="D6" s="27" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E6" s="27" t="s">
         <v>91</v>
@@ -1965,7 +1992,7 @@
       </c>
       <c r="C7" s="18"/>
       <c r="D7" s="16" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E7" s="19"/>
       <c r="F7" s="20" t="s">
@@ -1981,7 +2008,7 @@
       </c>
       <c r="C8" s="18"/>
       <c r="D8" s="16" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E8" s="21"/>
       <c r="F8" s="20" t="s">
@@ -1997,7 +2024,7 @@
       </c>
       <c r="C9" s="18"/>
       <c r="D9" s="23" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E9" s="18"/>
       <c r="F9" s="20" t="s">
@@ -2013,7 +2040,7 @@
       </c>
       <c r="C10" s="18"/>
       <c r="D10" s="23" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E10" s="21"/>
       <c r="F10" s="20" t="s">
@@ -2029,7 +2056,7 @@
       </c>
       <c r="C11" s="18"/>
       <c r="D11" s="16" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E11" s="18"/>
       <c r="F11" s="20" t="s">
@@ -2045,11 +2072,11 @@
       </c>
       <c r="C12" s="18"/>
       <c r="D12" s="23" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E12" s="28"/>
       <c r="F12" s="20" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -2061,7 +2088,7 @@
       </c>
       <c r="C13" s="18"/>
       <c r="D13" s="16" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E13" s="18"/>
       <c r="F13" s="20" t="s">
@@ -2077,7 +2104,7 @@
       </c>
       <c r="C14" s="18"/>
       <c r="D14" s="23" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E14" s="18"/>
       <c r="F14" s="20" t="s">
@@ -2093,7 +2120,7 @@
       </c>
       <c r="C15" s="18"/>
       <c r="D15" s="23" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E15" s="21"/>
       <c r="F15" s="20" t="s">
@@ -2109,7 +2136,7 @@
       </c>
       <c r="C16" s="18"/>
       <c r="D16" s="23" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E16" s="18"/>
       <c r="F16" s="20" t="s">
@@ -2125,7 +2152,7 @@
       </c>
       <c r="C17" s="18"/>
       <c r="D17" s="16" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E17" s="21"/>
       <c r="F17" s="20" t="s">
@@ -2141,7 +2168,7 @@
       </c>
       <c r="C18" s="18"/>
       <c r="D18" s="16" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E18" s="18"/>
       <c r="F18" s="20" t="s">
@@ -2157,7 +2184,7 @@
       </c>
       <c r="C19" s="18"/>
       <c r="D19" s="16" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E19" s="18"/>
       <c r="F19" s="20" t="s">
@@ -2173,7 +2200,7 @@
       </c>
       <c r="C20" s="18"/>
       <c r="D20" s="24" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E20" s="18"/>
       <c r="F20" s="20" t="s">
@@ -2189,7 +2216,7 @@
       </c>
       <c r="C21" s="18"/>
       <c r="D21" s="16" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E21" s="19"/>
       <c r="F21" s="20" t="s">
@@ -2205,11 +2232,11 @@
       </c>
       <c r="C22" s="18"/>
       <c r="D22" s="24" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E22" s="22"/>
       <c r="F22" s="20" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
@@ -2221,7 +2248,7 @@
       </c>
       <c r="C23" s="18"/>
       <c r="D23" s="17" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E23" s="19"/>
       <c r="F23" s="20" t="s">
@@ -2237,7 +2264,7 @@
       </c>
       <c r="C24" s="18"/>
       <c r="D24" s="17" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E24" s="19"/>
       <c r="F24" s="20" t="s">
@@ -2246,18 +2273,18 @@
     </row>
     <row r="25" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A25" s="20" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B25" s="18" t="s">
         <v>33</v>
       </c>
       <c r="C25" s="18"/>
       <c r="D25" s="29" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E25" s="18"/>
       <c r="F25" s="20" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
@@ -2269,14 +2296,14 @@
       </c>
       <c r="C26" s="18"/>
       <c r="D26" s="16" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E26" s="21"/>
       <c r="F26" s="20" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A27" s="18" t="s">
         <v>84</v>
       </c>
@@ -2285,11 +2312,11 @@
       </c>
       <c r="C27" s="18"/>
       <c r="D27" s="16" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E27" s="21"/>
       <c r="F27" s="20" t="s">
-        <v>108</v>
+        <v>170</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="115.2" x14ac:dyDescent="0.3">
@@ -2301,11 +2328,11 @@
       </c>
       <c r="C28" s="18"/>
       <c r="D28" s="16" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E28" s="21"/>
       <c r="F28" s="20" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="29" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -2317,11 +2344,11 @@
       </c>
       <c r="C29" s="18"/>
       <c r="D29" s="16" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E29" s="21"/>
       <c r="F29" s="20" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="30" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -2333,313 +2360,313 @@
       </c>
       <c r="C30" s="18"/>
       <c r="D30" s="16" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E30" s="18"/>
       <c r="F30" s="20" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" s="28" t="s">
+        <v>119</v>
+      </c>
+      <c r="B31" s="16" t="s">
         <v>120</v>
-      </c>
-      <c r="B31" s="16" t="s">
-        <v>121</v>
       </c>
       <c r="C31" s="16"/>
       <c r="D31" s="29" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E31" s="16"/>
       <c r="F31" s="30"/>
     </row>
     <row r="32" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A32" s="28" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B32" s="16" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C32" s="16" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D32" s="16" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E32" s="31"/>
       <c r="F32" s="30" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="33" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A33" s="28" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B33" s="16" t="s">
         <v>44</v>
       </c>
       <c r="C33" s="16" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D33" s="29" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E33" s="16"/>
       <c r="F33" s="30" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="34" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A34" s="28" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B34" s="16" t="s">
         <v>46</v>
       </c>
       <c r="C34" s="16" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D34" s="29" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E34" s="16"/>
       <c r="F34" s="30" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35" s="28" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B35" s="16" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C35" s="16"/>
       <c r="D35" s="16" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E35" s="16"/>
       <c r="F35" s="30" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="36" spans="1:6" ht="72" x14ac:dyDescent="0.3">
       <c r="A36" s="28" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B36" s="16" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C36" s="16" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D36" s="16" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E36" s="31"/>
       <c r="F36" s="30" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="37" spans="1:6" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A37" s="28" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B37" s="16" t="s">
         <v>51</v>
       </c>
       <c r="C37" s="16" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D37" s="33" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E37" s="31"/>
       <c r="F37" s="30" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38" s="28" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B38" s="16" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C38" s="16" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D38" s="16" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E38" s="16"/>
       <c r="F38" s="30" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39" s="28" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B39" s="16" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C39" s="16" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D39" s="16" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E39" s="16"/>
       <c r="F39" s="30" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A40" s="28"/>
       <c r="B40" s="16" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C40" s="16"/>
       <c r="D40" s="16"/>
       <c r="E40" s="16" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="F40" s="30"/>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A41" s="28" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B41" s="16" t="s">
         <v>45</v>
       </c>
       <c r="C41" s="16" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D41" s="29" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E41" s="16"/>
       <c r="F41" s="30" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="42" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A42" s="28" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B42" s="16" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C42" s="16" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D42" s="16" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E42" s="16"/>
       <c r="F42" s="30" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A43" s="28"/>
       <c r="B43" s="16" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C43" s="16" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D43" s="16" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E43" s="16"/>
       <c r="F43" s="30" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="44" spans="1:6" ht="72" x14ac:dyDescent="0.3">
       <c r="A44" s="28" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B44" s="16" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C44" s="16" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D44" s="16" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E44" s="31"/>
       <c r="F44" s="30" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A45" s="28" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B45" s="16" t="s">
         <v>47</v>
       </c>
       <c r="C45" s="16"/>
       <c r="D45" s="16" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E45" s="16"/>
       <c r="F45" s="30" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A46" s="28" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B46" s="16" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C46" s="16"/>
       <c r="D46" s="16" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E46" s="16"/>
       <c r="F46" s="30" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A47" s="28" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B47" s="16" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C47" s="16"/>
       <c r="D47" s="16" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E47" s="31"/>
       <c r="F47" s="30" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A48" s="28" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B48" s="16" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C48" s="16"/>
       <c r="D48" s="16" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E48" s="31"/>
       <c r="F48" s="30" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="74" spans="6:6" x14ac:dyDescent="0.3">
@@ -2711,25 +2738,35 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17E60BD9-E4DA-475A-8F4C-03B41D8829BF}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>163</v>
+      </c>
+      <c r="B3" t="s">
         <v>164</v>
       </c>
-      <c r="B3" t="s">
-        <v>165</v>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B4" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B5" t="s">
+        <v>169</v>
       </c>
     </row>
   </sheetData>
@@ -2859,7 +2896,7 @@
         <v>3</v>
       </c>
       <c r="G4" s="6">
-        <f t="shared" ref="G3:G66" si="0">DATE(B4,D4,1)</f>
+        <f t="shared" ref="G4:G66" si="0">DATE(B4,D4,1)</f>
         <v>33208</v>
       </c>
       <c r="H4">

</xml_diff>